<commit_message>
fix: removed password and added breakdown of ctc
</commit_message>
<xml_diff>
--- a/public/sample.xlsx
+++ b/public/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\arjunv\work\Placify\Placify.io\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\arjunv\work\Placify\Placify.io\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15250B0-5CFD-47F0-AAB3-C3CB35B9472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A5F5CC-E77D-486A-916E-1787791E9774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>username</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>accountType</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
 </sst>
 </file>
@@ -354,15 +351,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -372,9 +369,6 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: added student profile
</commit_message>
<xml_diff>
--- a/public/sample.xlsx
+++ b/public/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\arjunv\work\Placify\Placify.io\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB8FA2D-EB44-49EF-9783-11AB9DF5BD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58444610-4826-42B0-A342-C390DDC70FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -34,6 +34,33 @@
   </si>
   <si>
     <t>studentName</t>
+  </si>
+  <si>
+    <t>contactNo</t>
+  </si>
+  <si>
+    <t>studentTenthMarks</t>
+  </si>
+  <si>
+    <t>studentTwelthMarks</t>
+  </si>
+  <si>
+    <t>studentUGMarks</t>
+  </si>
+  <si>
+    <t>studentPGMarks</t>
+  </si>
+  <si>
+    <t>studentDescription</t>
+  </si>
+  <si>
+    <t>studentId</t>
+  </si>
+  <si>
+    <t>dept</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
@@ -351,15 +378,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -368,6 +395,33 @@
       </c>
       <c r="C1" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>